<commit_message>
:memo: add modif (#33)
</commit_message>
<xml_diff>
--- a/Documents/Benefices_Production_Soupe_Théorique.xlsx
+++ b/Documents/Benefices_Production_Soupe_Théorique.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\chronobio-client\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\chronobio-client-1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EC8AD3-A40E-4A89-BEA9-98EE8903413A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBBAC6E-8DFC-423D-9108-4F3805F3066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,7 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1087,25 +1087,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1186,34 +1186,33 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -1248,12 +1247,12 @@
       <sheetName val="gestion emprunt"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="9">
           <cell r="J9">
@@ -1571,7 +1570,7 @@
   <dimension ref="A2:BR175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1658,7 @@
       <c r="V3" s="86"/>
       <c r="W3" s="87"/>
       <c r="X3" s="1">
-        <v>98000</v>
+        <v>106000</v>
       </c>
       <c r="AE3" s="88" t="s">
         <v>21</v>
@@ -1709,7 +1708,7 @@
       <c r="V5" s="98"/>
       <c r="W5" s="103">
         <f>X3/3</f>
-        <v>32666.666666666668</v>
+        <v>35333.333333333336</v>
       </c>
       <c r="X5" s="104"/>
       <c r="AE5" s="91"/>
@@ -1772,7 +1771,7 @@
       <c r="V6" s="100"/>
       <c r="W6" s="99">
         <f>X3/4</f>
-        <v>24500</v>
+        <v>26500</v>
       </c>
       <c r="X6" s="100"/>
       <c r="AE6" s="91"/>
@@ -1840,7 +1839,7 @@
       <c r="V7" s="102"/>
       <c r="W7" s="101">
         <f>X3/5</f>
-        <v>19600</v>
+        <v>21200</v>
       </c>
       <c r="X7" s="102"/>
       <c r="AE7" s="94"/>
@@ -2253,10 +2252,10 @@
         <f t="shared" ref="AB13:AB16" si="9">Z13*5</f>
         <v>360000</v>
       </c>
-      <c r="AE13" s="108">
+      <c r="AE13" s="106">
         <v>8</v>
       </c>
-      <c r="AF13" s="78">
+      <c r="AF13" s="107">
         <v>1</v>
       </c>
       <c r="AG13" s="20">
@@ -2273,7 +2272,7 @@
         <f>$O$14-AH13</f>
         <v>184000</v>
       </c>
-      <c r="AK13" s="109">
+      <c r="AK13" s="108">
         <v>33</v>
       </c>
       <c r="AL13" s="105">
@@ -2367,8 +2366,8 @@
         <f t="shared" si="9"/>
         <v>720000</v>
       </c>
-      <c r="AE14" s="108"/>
-      <c r="AF14" s="78"/>
+      <c r="AE14" s="106"/>
+      <c r="AF14" s="107"/>
       <c r="AG14" s="20">
         <v>2</v>
       </c>
@@ -2383,8 +2382,8 @@
         <f>$O$14-AH14</f>
         <v>183920</v>
       </c>
-      <c r="AK14" s="109"/>
-      <c r="AL14" s="106"/>
+      <c r="AK14" s="108"/>
+      <c r="AL14" s="74"/>
       <c r="AM14" s="24">
         <v>2</v>
       </c>
@@ -2473,8 +2472,8 @@
         <f t="shared" si="9"/>
         <v>1080000</v>
       </c>
-      <c r="AE15" s="108"/>
-      <c r="AF15" s="78"/>
+      <c r="AE15" s="106"/>
+      <c r="AF15" s="107"/>
       <c r="AG15" s="20">
         <v>3</v>
       </c>
@@ -2489,8 +2488,8 @@
         <f t="shared" ref="AJ15:AJ72" si="11">$O$14-AH15</f>
         <v>183839.2</v>
       </c>
-      <c r="AK15" s="109"/>
-      <c r="AL15" s="106"/>
+      <c r="AK15" s="108"/>
+      <c r="AL15" s="74"/>
       <c r="AM15" s="24">
         <v>3</v>
       </c>
@@ -2579,8 +2578,8 @@
         <f t="shared" si="9"/>
         <v>1440000</v>
       </c>
-      <c r="AE16" s="108"/>
-      <c r="AF16" s="78"/>
+      <c r="AE16" s="106"/>
+      <c r="AF16" s="107"/>
       <c r="AG16" s="20">
         <v>4</v>
       </c>
@@ -2595,8 +2594,8 @@
         <f t="shared" si="11"/>
         <v>183757.592</v>
       </c>
-      <c r="AK16" s="109"/>
-      <c r="AL16" s="106"/>
+      <c r="AK16" s="108"/>
+      <c r="AL16" s="74"/>
       <c r="AM16" s="24">
         <v>4</v>
       </c>
@@ -2658,8 +2657,8 @@
         <f t="shared" si="5"/>
         <v>264000</v>
       </c>
-      <c r="AE17" s="108"/>
-      <c r="AF17" s="78"/>
+      <c r="AE17" s="106"/>
+      <c r="AF17" s="107"/>
       <c r="AG17" s="20">
         <v>5</v>
       </c>
@@ -2674,8 +2673,8 @@
         <f t="shared" si="11"/>
         <v>183675.16792000001</v>
       </c>
-      <c r="AK17" s="109"/>
-      <c r="AL17" s="106"/>
+      <c r="AK17" s="108"/>
+      <c r="AL17" s="74"/>
       <c r="AM17" s="24">
         <v>5</v>
       </c>
@@ -2737,8 +2736,8 @@
         <f t="shared" si="5"/>
         <v>288000</v>
       </c>
-      <c r="AE18" s="108"/>
-      <c r="AF18" s="78"/>
+      <c r="AE18" s="106"/>
+      <c r="AF18" s="107"/>
       <c r="AG18" s="20">
         <v>6</v>
       </c>
@@ -2753,8 +2752,8 @@
         <f t="shared" si="11"/>
         <v>183591.91959919999</v>
       </c>
-      <c r="AK18" s="109"/>
-      <c r="AL18" s="106"/>
+      <c r="AK18" s="108"/>
+      <c r="AL18" s="74"/>
       <c r="AM18" s="24">
         <v>6</v>
       </c>
@@ -2816,8 +2815,8 @@
         <f t="shared" si="5"/>
         <v>312000</v>
       </c>
-      <c r="AE19" s="108"/>
-      <c r="AF19" s="78"/>
+      <c r="AE19" s="106"/>
+      <c r="AF19" s="107"/>
       <c r="AG19" s="20">
         <v>7</v>
       </c>
@@ -2832,8 +2831,8 @@
         <f t="shared" si="11"/>
         <v>183507.83879519202</v>
       </c>
-      <c r="AK19" s="109"/>
-      <c r="AL19" s="106"/>
+      <c r="AK19" s="108"/>
+      <c r="AL19" s="74"/>
       <c r="AM19" s="24">
         <v>7</v>
       </c>
@@ -2895,8 +2894,8 @@
         <f t="shared" si="5"/>
         <v>336000</v>
       </c>
-      <c r="AE20" s="108"/>
-      <c r="AF20" s="78"/>
+      <c r="AE20" s="106"/>
+      <c r="AF20" s="107"/>
       <c r="AG20" s="20">
         <v>8</v>
       </c>
@@ -2911,8 +2910,8 @@
         <f t="shared" si="11"/>
         <v>183422.91718314393</v>
       </c>
-      <c r="AK20" s="109"/>
-      <c r="AL20" s="106"/>
+      <c r="AK20" s="108"/>
+      <c r="AL20" s="74"/>
       <c r="AM20" s="24">
         <v>8</v>
       </c>
@@ -2974,8 +2973,8 @@
         <f t="shared" si="5"/>
         <v>360000</v>
       </c>
-      <c r="AE21" s="108"/>
-      <c r="AF21" s="78"/>
+      <c r="AE21" s="106"/>
+      <c r="AF21" s="107"/>
       <c r="AG21" s="20">
         <v>9</v>
       </c>
@@ -2990,8 +2989,8 @@
         <f t="shared" si="11"/>
         <v>183337.14635497535</v>
       </c>
-      <c r="AK21" s="109"/>
-      <c r="AL21" s="106"/>
+      <c r="AK21" s="108"/>
+      <c r="AL21" s="74"/>
       <c r="AM21" s="24">
         <v>9</v>
       </c>
@@ -3053,8 +3052,8 @@
         <f t="shared" si="5"/>
         <v>384000</v>
       </c>
-      <c r="AE22" s="108"/>
-      <c r="AF22" s="78"/>
+      <c r="AE22" s="106"/>
+      <c r="AF22" s="107"/>
       <c r="AG22" s="20">
         <v>10</v>
       </c>
@@ -3069,8 +3068,8 @@
         <f t="shared" si="11"/>
         <v>183250.51781852511</v>
       </c>
-      <c r="AK22" s="109"/>
-      <c r="AL22" s="106"/>
+      <c r="AK22" s="108"/>
+      <c r="AL22" s="74"/>
       <c r="AM22" s="24">
         <v>10</v>
       </c>
@@ -3132,13 +3131,8 @@
         <f t="shared" si="5"/>
         <v>408000</v>
       </c>
-      <c r="U23" s="115"/>
-      <c r="V23" s="115"/>
-      <c r="W23" s="115"/>
-      <c r="X23" s="115"/>
-      <c r="Y23" s="115"/>
-      <c r="AE23" s="108"/>
-      <c r="AF23" s="78"/>
+      <c r="AE23" s="106"/>
+      <c r="AF23" s="107"/>
       <c r="AG23" s="20">
         <v>11</v>
       </c>
@@ -3153,8 +3147,8 @@
         <f t="shared" si="11"/>
         <v>183163.02299671035</v>
       </c>
-      <c r="AK23" s="109"/>
-      <c r="AL23" s="106"/>
+      <c r="AK23" s="108"/>
+      <c r="AL23" s="74"/>
       <c r="AM23" s="24">
         <v>11</v>
       </c>
@@ -3216,13 +3210,8 @@
         <f t="shared" si="5"/>
         <v>432000</v>
       </c>
-      <c r="U24" s="115"/>
-      <c r="V24" s="115"/>
-      <c r="W24" s="115"/>
-      <c r="X24" s="115"/>
-      <c r="Y24" s="115"/>
-      <c r="AE24" s="108"/>
-      <c r="AF24" s="78"/>
+      <c r="AE24" s="106"/>
+      <c r="AF24" s="107"/>
       <c r="AG24" s="20">
         <v>12</v>
       </c>
@@ -3237,8 +3226,8 @@
         <f t="shared" si="11"/>
         <v>183074.65322667747</v>
       </c>
-      <c r="AK24" s="109"/>
-      <c r="AL24" s="107"/>
+      <c r="AK24" s="108"/>
+      <c r="AL24" s="75"/>
       <c r="AM24" s="24">
         <v>12</v>
       </c>
@@ -3300,13 +3289,8 @@
         <f t="shared" si="5"/>
         <v>456000</v>
       </c>
-      <c r="U25" s="115"/>
-      <c r="V25" s="115"/>
-      <c r="W25" s="115"/>
-      <c r="X25" s="115"/>
-      <c r="Y25" s="115"/>
-      <c r="AE25" s="108"/>
-      <c r="AF25" s="78">
+      <c r="AE25" s="106"/>
+      <c r="AF25" s="107">
         <v>2</v>
       </c>
       <c r="AG25" s="20">
@@ -3323,8 +3307,8 @@
         <f t="shared" si="11"/>
         <v>182985.39975894423</v>
       </c>
-      <c r="AK25" s="109"/>
-      <c r="AL25" s="110">
+      <c r="AK25" s="108"/>
+      <c r="AL25" s="73">
         <v>2</v>
       </c>
       <c r="AM25" s="24">
@@ -3388,13 +3372,8 @@
         <f t="shared" si="5"/>
         <v>480000</v>
       </c>
-      <c r="U26" s="115"/>
-      <c r="V26" s="115"/>
-      <c r="W26" s="115"/>
-      <c r="X26" s="115"/>
-      <c r="Y26" s="115"/>
-      <c r="AE26" s="108"/>
-      <c r="AF26" s="78"/>
+      <c r="AE26" s="106"/>
+      <c r="AF26" s="107"/>
       <c r="AG26" s="20">
         <v>14</v>
       </c>
@@ -3409,8 +3388,8 @@
         <f t="shared" si="11"/>
         <v>182895.2537565337</v>
       </c>
-      <c r="AK26" s="109"/>
-      <c r="AL26" s="106"/>
+      <c r="AK26" s="108"/>
+      <c r="AL26" s="74"/>
       <c r="AM26" s="24">
         <v>14</v>
       </c>
@@ -3472,13 +3451,8 @@
         <f t="shared" si="5"/>
         <v>504000</v>
       </c>
-      <c r="U27" s="115"/>
-      <c r="V27" s="115"/>
-      <c r="W27" s="115"/>
-      <c r="X27" s="115"/>
-      <c r="Y27" s="115"/>
-      <c r="AE27" s="108"/>
-      <c r="AF27" s="78"/>
+      <c r="AE27" s="106"/>
+      <c r="AF27" s="107"/>
       <c r="AG27" s="20">
         <v>15</v>
       </c>
@@ -3493,8 +3467,8 @@
         <f t="shared" si="11"/>
         <v>182804.20629409901</v>
       </c>
-      <c r="AK27" s="109"/>
-      <c r="AL27" s="106"/>
+      <c r="AK27" s="108"/>
+      <c r="AL27" s="74"/>
       <c r="AM27" s="24">
         <v>15</v>
       </c>
@@ -3556,13 +3530,8 @@
         <f t="shared" si="5"/>
         <v>528000</v>
       </c>
-      <c r="U28" s="115"/>
-      <c r="V28" s="115"/>
-      <c r="W28" s="115"/>
-      <c r="X28" s="115"/>
-      <c r="Y28" s="115"/>
-      <c r="AE28" s="108"/>
-      <c r="AF28" s="78"/>
+      <c r="AE28" s="106"/>
+      <c r="AF28" s="107"/>
       <c r="AG28" s="20">
         <v>16</v>
       </c>
@@ -3577,8 +3546,8 @@
         <f t="shared" si="11"/>
         <v>184000</v>
       </c>
-      <c r="AK28" s="109"/>
-      <c r="AL28" s="106"/>
+      <c r="AK28" s="108"/>
+      <c r="AL28" s="74"/>
       <c r="AM28" s="27">
         <v>16</v>
       </c>
@@ -3640,8 +3609,8 @@
         <f t="shared" si="5"/>
         <v>552000</v>
       </c>
-      <c r="AE29" s="108"/>
-      <c r="AF29" s="78"/>
+      <c r="AE29" s="106"/>
+      <c r="AF29" s="107"/>
       <c r="AG29" s="20">
         <v>17</v>
       </c>
@@ -3656,8 +3625,8 @@
         <f t="shared" si="11"/>
         <v>183920</v>
       </c>
-      <c r="AK29" s="109"/>
-      <c r="AL29" s="106"/>
+      <c r="AK29" s="108"/>
+      <c r="AL29" s="74"/>
       <c r="AM29" s="27">
         <v>17</v>
       </c>
@@ -3719,8 +3688,8 @@
         <f t="shared" si="5"/>
         <v>576000</v>
       </c>
-      <c r="AE30" s="108"/>
-      <c r="AF30" s="78"/>
+      <c r="AE30" s="106"/>
+      <c r="AF30" s="107"/>
       <c r="AG30" s="20">
         <v>18</v>
       </c>
@@ -3735,8 +3704,8 @@
         <f t="shared" si="11"/>
         <v>183839.2</v>
       </c>
-      <c r="AK30" s="109"/>
-      <c r="AL30" s="106"/>
+      <c r="AK30" s="108"/>
+      <c r="AL30" s="74"/>
       <c r="AM30" s="27">
         <v>18</v>
       </c>
@@ -3798,8 +3767,8 @@
         <f t="shared" si="5"/>
         <v>600000</v>
       </c>
-      <c r="AE31" s="108"/>
-      <c r="AF31" s="78"/>
+      <c r="AE31" s="106"/>
+      <c r="AF31" s="107"/>
       <c r="AG31" s="20">
         <v>19</v>
       </c>
@@ -3814,8 +3783,8 @@
         <f t="shared" si="11"/>
         <v>183757.592</v>
       </c>
-      <c r="AK31" s="109"/>
-      <c r="AL31" s="106"/>
+      <c r="AK31" s="108"/>
+      <c r="AL31" s="74"/>
       <c r="AM31" s="27">
         <v>19</v>
       </c>
@@ -3877,8 +3846,8 @@
         <f t="shared" si="5"/>
         <v>624000</v>
       </c>
-      <c r="AE32" s="108"/>
-      <c r="AF32" s="78"/>
+      <c r="AE32" s="106"/>
+      <c r="AF32" s="107"/>
       <c r="AG32" s="20">
         <v>20</v>
       </c>
@@ -3893,8 +3862,8 @@
         <f t="shared" si="11"/>
         <v>183675.16792000001</v>
       </c>
-      <c r="AK32" s="109"/>
-      <c r="AL32" s="106"/>
+      <c r="AK32" s="108"/>
+      <c r="AL32" s="74"/>
       <c r="AM32" s="27">
         <v>20</v>
       </c>
@@ -3956,8 +3925,8 @@
         <f t="shared" si="5"/>
         <v>648000</v>
       </c>
-      <c r="AE33" s="108"/>
-      <c r="AF33" s="78"/>
+      <c r="AE33" s="106"/>
+      <c r="AF33" s="107"/>
       <c r="AG33" s="20">
         <v>21</v>
       </c>
@@ -3972,8 +3941,8 @@
         <f t="shared" si="11"/>
         <v>183591.91959919999</v>
       </c>
-      <c r="AK33" s="109"/>
-      <c r="AL33" s="106"/>
+      <c r="AK33" s="108"/>
+      <c r="AL33" s="74"/>
       <c r="AM33" s="27">
         <v>21</v>
       </c>
@@ -4035,8 +4004,8 @@
         <f t="shared" si="5"/>
         <v>672000</v>
       </c>
-      <c r="AE34" s="108"/>
-      <c r="AF34" s="78"/>
+      <c r="AE34" s="106"/>
+      <c r="AF34" s="107"/>
       <c r="AG34" s="20">
         <v>22</v>
       </c>
@@ -4051,8 +4020,8 @@
         <f t="shared" si="11"/>
         <v>183507.83879519202</v>
       </c>
-      <c r="AK34" s="109"/>
-      <c r="AL34" s="106"/>
+      <c r="AK34" s="108"/>
+      <c r="AL34" s="74"/>
       <c r="AM34" s="27">
         <v>22</v>
       </c>
@@ -4114,8 +4083,8 @@
         <f t="shared" si="5"/>
         <v>696000</v>
       </c>
-      <c r="AE35" s="108"/>
-      <c r="AF35" s="78"/>
+      <c r="AE35" s="106"/>
+      <c r="AF35" s="107"/>
       <c r="AG35" s="20">
         <v>23</v>
       </c>
@@ -4130,8 +4099,8 @@
         <f t="shared" si="11"/>
         <v>183422.91718314393</v>
       </c>
-      <c r="AK35" s="109"/>
-      <c r="AL35" s="106"/>
+      <c r="AK35" s="108"/>
+      <c r="AL35" s="74"/>
       <c r="AM35" s="27">
         <v>23</v>
       </c>
@@ -4193,8 +4162,8 @@
         <f t="shared" si="5"/>
         <v>720000</v>
       </c>
-      <c r="AE36" s="108"/>
-      <c r="AF36" s="78"/>
+      <c r="AE36" s="106"/>
+      <c r="AF36" s="107"/>
       <c r="AG36" s="20">
         <v>24</v>
       </c>
@@ -4209,8 +4178,8 @@
         <f t="shared" si="11"/>
         <v>183337.14635497535</v>
       </c>
-      <c r="AK36" s="109"/>
-      <c r="AL36" s="107"/>
+      <c r="AK36" s="108"/>
+      <c r="AL36" s="75"/>
       <c r="AM36" s="27">
         <v>24</v>
       </c>
@@ -4272,8 +4241,8 @@
         <f t="shared" si="5"/>
         <v>744000</v>
       </c>
-      <c r="AE37" s="108"/>
-      <c r="AF37" s="78">
+      <c r="AE37" s="106"/>
+      <c r="AF37" s="107">
         <v>3</v>
       </c>
       <c r="AG37" s="20">
@@ -4290,8 +4259,8 @@
         <f t="shared" si="11"/>
         <v>183250.51781852511</v>
       </c>
-      <c r="AK37" s="109"/>
-      <c r="AL37" s="110">
+      <c r="AK37" s="108"/>
+      <c r="AL37" s="73">
         <v>3</v>
       </c>
       <c r="AM37" s="27">
@@ -4355,8 +4324,8 @@
         <f t="shared" si="5"/>
         <v>768000</v>
       </c>
-      <c r="AE38" s="108"/>
-      <c r="AF38" s="78"/>
+      <c r="AE38" s="106"/>
+      <c r="AF38" s="107"/>
       <c r="AG38" s="20">
         <v>26</v>
       </c>
@@ -4371,8 +4340,8 @@
         <f t="shared" si="11"/>
         <v>183163.02299671035</v>
       </c>
-      <c r="AK38" s="109"/>
-      <c r="AL38" s="106"/>
+      <c r="AK38" s="108"/>
+      <c r="AL38" s="74"/>
       <c r="AM38" s="27">
         <v>26</v>
       </c>
@@ -4434,8 +4403,8 @@
         <f t="shared" si="5"/>
         <v>792000</v>
       </c>
-      <c r="AE39" s="108"/>
-      <c r="AF39" s="78"/>
+      <c r="AE39" s="106"/>
+      <c r="AF39" s="107"/>
       <c r="AG39" s="20">
         <v>27</v>
       </c>
@@ -4450,8 +4419,8 @@
         <f t="shared" si="11"/>
         <v>183074.65322667747</v>
       </c>
-      <c r="AK39" s="109"/>
-      <c r="AL39" s="106"/>
+      <c r="AK39" s="108"/>
+      <c r="AL39" s="74"/>
       <c r="AM39" s="27">
         <v>27</v>
       </c>
@@ -4513,8 +4482,8 @@
         <f t="shared" si="5"/>
         <v>816000</v>
       </c>
-      <c r="AE40" s="108"/>
-      <c r="AF40" s="78"/>
+      <c r="AE40" s="106"/>
+      <c r="AF40" s="107"/>
       <c r="AG40" s="20">
         <v>28</v>
       </c>
@@ -4529,8 +4498,8 @@
         <f t="shared" si="11"/>
         <v>182985.39975894423</v>
       </c>
-      <c r="AK40" s="109"/>
-      <c r="AL40" s="106"/>
+      <c r="AK40" s="108"/>
+      <c r="AL40" s="74"/>
       <c r="AM40" s="27">
         <v>28</v>
       </c>
@@ -4592,8 +4561,8 @@
         <f t="shared" si="5"/>
         <v>840000</v>
       </c>
-      <c r="AE41" s="108"/>
-      <c r="AF41" s="78"/>
+      <c r="AE41" s="106"/>
+      <c r="AF41" s="107"/>
       <c r="AG41" s="20">
         <v>29</v>
       </c>
@@ -4608,8 +4577,8 @@
         <f t="shared" si="11"/>
         <v>182895.2537565337</v>
       </c>
-      <c r="AK41" s="109"/>
-      <c r="AL41" s="106"/>
+      <c r="AK41" s="108"/>
+      <c r="AL41" s="74"/>
       <c r="AM41" s="27">
         <v>29</v>
       </c>
@@ -4671,8 +4640,8 @@
         <f t="shared" si="5"/>
         <v>864000</v>
       </c>
-      <c r="AE42" s="108"/>
-      <c r="AF42" s="78"/>
+      <c r="AE42" s="106"/>
+      <c r="AF42" s="107"/>
       <c r="AG42" s="20">
         <v>30</v>
       </c>
@@ -4687,8 +4656,8 @@
         <f t="shared" si="11"/>
         <v>182804.20629409901</v>
       </c>
-      <c r="AK42" s="109"/>
-      <c r="AL42" s="106"/>
+      <c r="AK42" s="108"/>
+      <c r="AL42" s="74"/>
       <c r="AM42" s="27">
         <v>30</v>
       </c>
@@ -4750,8 +4719,8 @@
         <f t="shared" si="5"/>
         <v>888000</v>
       </c>
-      <c r="AE43" s="108"/>
-      <c r="AF43" s="78"/>
+      <c r="AE43" s="106"/>
+      <c r="AF43" s="107"/>
       <c r="AG43" s="20">
         <v>31</v>
       </c>
@@ -4766,8 +4735,8 @@
         <f t="shared" si="11"/>
         <v>184000</v>
       </c>
-      <c r="AK43" s="109"/>
-      <c r="AL43" s="106"/>
+      <c r="AK43" s="108"/>
+      <c r="AL43" s="74"/>
       <c r="AM43" s="24">
         <v>31</v>
       </c>
@@ -4829,8 +4798,8 @@
         <f t="shared" si="5"/>
         <v>912000</v>
       </c>
-      <c r="AE44" s="108"/>
-      <c r="AF44" s="78"/>
+      <c r="AE44" s="106"/>
+      <c r="AF44" s="107"/>
       <c r="AG44" s="20">
         <v>32</v>
       </c>
@@ -4845,8 +4814,8 @@
         <f t="shared" si="11"/>
         <v>183920</v>
       </c>
-      <c r="AK44" s="109"/>
-      <c r="AL44" s="106"/>
+      <c r="AK44" s="108"/>
+      <c r="AL44" s="74"/>
       <c r="AM44" s="24">
         <v>32</v>
       </c>
@@ -4908,8 +4877,8 @@
         <f t="shared" si="5"/>
         <v>936000</v>
       </c>
-      <c r="AE45" s="108"/>
-      <c r="AF45" s="78"/>
+      <c r="AE45" s="106"/>
+      <c r="AF45" s="107"/>
       <c r="AG45" s="20">
         <v>33</v>
       </c>
@@ -4924,8 +4893,8 @@
         <f t="shared" si="11"/>
         <v>183839.2</v>
       </c>
-      <c r="AK45" s="109"/>
-      <c r="AL45" s="106"/>
+      <c r="AK45" s="108"/>
+      <c r="AL45" s="74"/>
       <c r="AM45" s="24">
         <v>33</v>
       </c>
@@ -4987,8 +4956,8 @@
         <f t="shared" si="5"/>
         <v>960000</v>
       </c>
-      <c r="AE46" s="108"/>
-      <c r="AF46" s="78"/>
+      <c r="AE46" s="106"/>
+      <c r="AF46" s="107"/>
       <c r="AG46" s="20">
         <v>34</v>
       </c>
@@ -5003,8 +4972,8 @@
         <f t="shared" si="11"/>
         <v>183757.592</v>
       </c>
-      <c r="AK46" s="109"/>
-      <c r="AL46" s="106"/>
+      <c r="AK46" s="108"/>
+      <c r="AL46" s="74"/>
       <c r="AM46" s="24">
         <v>34</v>
       </c>
@@ -5066,8 +5035,8 @@
         <f t="shared" si="5"/>
         <v>984000</v>
       </c>
-      <c r="AE47" s="108"/>
-      <c r="AF47" s="78"/>
+      <c r="AE47" s="106"/>
+      <c r="AF47" s="107"/>
       <c r="AG47" s="20">
         <v>35</v>
       </c>
@@ -5082,8 +5051,8 @@
         <f t="shared" si="11"/>
         <v>183675.16792000001</v>
       </c>
-      <c r="AK47" s="109"/>
-      <c r="AL47" s="106"/>
+      <c r="AK47" s="108"/>
+      <c r="AL47" s="74"/>
       <c r="AM47" s="24">
         <v>35</v>
       </c>
@@ -5145,8 +5114,8 @@
         <f t="shared" si="5"/>
         <v>1008000</v>
       </c>
-      <c r="AE48" s="108"/>
-      <c r="AF48" s="78"/>
+      <c r="AE48" s="106"/>
+      <c r="AF48" s="107"/>
       <c r="AG48" s="20">
         <v>36</v>
       </c>
@@ -5161,8 +5130,8 @@
         <f t="shared" si="11"/>
         <v>183591.91959919999</v>
       </c>
-      <c r="AK48" s="109"/>
-      <c r="AL48" s="107"/>
+      <c r="AK48" s="108"/>
+      <c r="AL48" s="75"/>
       <c r="AM48" s="24">
         <v>36</v>
       </c>
@@ -5224,8 +5193,8 @@
         <f t="shared" si="5"/>
         <v>1032000</v>
       </c>
-      <c r="AE49" s="108"/>
-      <c r="AF49" s="78">
+      <c r="AE49" s="106"/>
+      <c r="AF49" s="107">
         <v>4</v>
       </c>
       <c r="AG49" s="20">
@@ -5242,8 +5211,8 @@
         <f t="shared" si="11"/>
         <v>183507.83879519202</v>
       </c>
-      <c r="AK49" s="109"/>
-      <c r="AL49" s="110">
+      <c r="AK49" s="108"/>
+      <c r="AL49" s="73">
         <v>4</v>
       </c>
       <c r="AM49" s="24">
@@ -5307,8 +5276,8 @@
         <f t="shared" si="5"/>
         <v>1056000</v>
       </c>
-      <c r="AE50" s="108"/>
-      <c r="AF50" s="78"/>
+      <c r="AE50" s="106"/>
+      <c r="AF50" s="107"/>
       <c r="AG50" s="20">
         <v>38</v>
       </c>
@@ -5323,8 +5292,8 @@
         <f t="shared" si="11"/>
         <v>183422.91718314393</v>
       </c>
-      <c r="AK50" s="109"/>
-      <c r="AL50" s="106"/>
+      <c r="AK50" s="108"/>
+      <c r="AL50" s="74"/>
       <c r="AM50" s="24">
         <v>38</v>
       </c>
@@ -5386,8 +5355,8 @@
         <f t="shared" si="5"/>
         <v>1080000</v>
       </c>
-      <c r="AE51" s="108"/>
-      <c r="AF51" s="78"/>
+      <c r="AE51" s="106"/>
+      <c r="AF51" s="107"/>
       <c r="AG51" s="20">
         <v>39</v>
       </c>
@@ -5402,8 +5371,8 @@
         <f t="shared" si="11"/>
         <v>183337.14635497535</v>
       </c>
-      <c r="AK51" s="109"/>
-      <c r="AL51" s="106"/>
+      <c r="AK51" s="108"/>
+      <c r="AL51" s="74"/>
       <c r="AM51" s="24">
         <v>39</v>
       </c>
@@ -5465,8 +5434,8 @@
         <f t="shared" si="5"/>
         <v>1104000</v>
       </c>
-      <c r="AE52" s="108"/>
-      <c r="AF52" s="78"/>
+      <c r="AE52" s="106"/>
+      <c r="AF52" s="107"/>
       <c r="AG52" s="20">
         <v>40</v>
       </c>
@@ -5481,8 +5450,8 @@
         <f t="shared" si="11"/>
         <v>183250.51781852511</v>
       </c>
-      <c r="AK52" s="109"/>
-      <c r="AL52" s="106"/>
+      <c r="AK52" s="108"/>
+      <c r="AL52" s="74"/>
       <c r="AM52" s="24">
         <v>40</v>
       </c>
@@ -5544,8 +5513,8 @@
         <f t="shared" si="5"/>
         <v>1128000</v>
       </c>
-      <c r="AE53" s="108"/>
-      <c r="AF53" s="78"/>
+      <c r="AE53" s="106"/>
+      <c r="AF53" s="107"/>
       <c r="AG53" s="20">
         <v>41</v>
       </c>
@@ -5560,8 +5529,8 @@
         <f t="shared" si="11"/>
         <v>183163.02299671035</v>
       </c>
-      <c r="AK53" s="109"/>
-      <c r="AL53" s="106"/>
+      <c r="AK53" s="108"/>
+      <c r="AL53" s="74"/>
       <c r="AM53" s="24">
         <v>41</v>
       </c>
@@ -5623,8 +5592,8 @@
         <f t="shared" si="5"/>
         <v>1152000</v>
       </c>
-      <c r="AE54" s="108"/>
-      <c r="AF54" s="78"/>
+      <c r="AE54" s="106"/>
+      <c r="AF54" s="107"/>
       <c r="AG54" s="20">
         <v>42</v>
       </c>
@@ -5639,8 +5608,8 @@
         <f t="shared" si="11"/>
         <v>183074.65322667747</v>
       </c>
-      <c r="AK54" s="109"/>
-      <c r="AL54" s="106"/>
+      <c r="AK54" s="108"/>
+      <c r="AL54" s="74"/>
       <c r="AM54" s="24">
         <v>42</v>
       </c>
@@ -5702,8 +5671,8 @@
         <f t="shared" si="5"/>
         <v>1176000</v>
       </c>
-      <c r="AE55" s="108"/>
-      <c r="AF55" s="78"/>
+      <c r="AE55" s="106"/>
+      <c r="AF55" s="107"/>
       <c r="AG55" s="20">
         <v>43</v>
       </c>
@@ -5718,8 +5687,8 @@
         <f t="shared" si="11"/>
         <v>182985.39975894423</v>
       </c>
-      <c r="AK55" s="109"/>
-      <c r="AL55" s="106"/>
+      <c r="AK55" s="108"/>
+      <c r="AL55" s="74"/>
       <c r="AM55" s="24">
         <v>43</v>
       </c>
@@ -5781,8 +5750,8 @@
         <f t="shared" si="5"/>
         <v>1200000</v>
       </c>
-      <c r="AE56" s="108"/>
-      <c r="AF56" s="78"/>
+      <c r="AE56" s="106"/>
+      <c r="AF56" s="107"/>
       <c r="AG56" s="20">
         <v>44</v>
       </c>
@@ -5797,8 +5766,8 @@
         <f t="shared" si="11"/>
         <v>182895.2537565337</v>
       </c>
-      <c r="AK56" s="109"/>
-      <c r="AL56" s="106"/>
+      <c r="AK56" s="108"/>
+      <c r="AL56" s="74"/>
       <c r="AM56" s="24">
         <v>44</v>
       </c>
@@ -5860,8 +5829,8 @@
         <f t="shared" si="5"/>
         <v>1224000</v>
       </c>
-      <c r="AE57" s="108"/>
-      <c r="AF57" s="78"/>
+      <c r="AE57" s="106"/>
+      <c r="AF57" s="107"/>
       <c r="AG57" s="20">
         <v>45</v>
       </c>
@@ -5876,8 +5845,8 @@
         <f t="shared" si="11"/>
         <v>182804.20629409901</v>
       </c>
-      <c r="AK57" s="109"/>
-      <c r="AL57" s="106"/>
+      <c r="AK57" s="108"/>
+      <c r="AL57" s="74"/>
       <c r="AM57" s="24">
         <v>45</v>
       </c>
@@ -5939,8 +5908,8 @@
         <f t="shared" si="5"/>
         <v>1248000</v>
       </c>
-      <c r="AE58" s="108"/>
-      <c r="AF58" s="78"/>
+      <c r="AE58" s="106"/>
+      <c r="AF58" s="107"/>
       <c r="AG58" s="20">
         <v>46</v>
       </c>
@@ -5955,8 +5924,8 @@
         <f t="shared" si="11"/>
         <v>184000</v>
       </c>
-      <c r="AK58" s="109"/>
-      <c r="AL58" s="106"/>
+      <c r="AK58" s="108"/>
+      <c r="AL58" s="74"/>
       <c r="AM58" s="27">
         <v>46</v>
       </c>
@@ -6018,8 +5987,8 @@
         <f t="shared" si="5"/>
         <v>1272000</v>
       </c>
-      <c r="AE59" s="108"/>
-      <c r="AF59" s="78"/>
+      <c r="AE59" s="106"/>
+      <c r="AF59" s="107"/>
       <c r="AG59" s="20">
         <v>47</v>
       </c>
@@ -6034,8 +6003,8 @@
         <f t="shared" si="11"/>
         <v>183920</v>
       </c>
-      <c r="AK59" s="109"/>
-      <c r="AL59" s="106"/>
+      <c r="AK59" s="108"/>
+      <c r="AL59" s="74"/>
       <c r="AM59" s="27">
         <v>47</v>
       </c>
@@ -6097,8 +6066,8 @@
         <f t="shared" si="5"/>
         <v>1296000</v>
       </c>
-      <c r="AE60" s="108"/>
-      <c r="AF60" s="78"/>
+      <c r="AE60" s="106"/>
+      <c r="AF60" s="107"/>
       <c r="AG60" s="20">
         <v>48</v>
       </c>
@@ -6113,8 +6082,8 @@
         <f t="shared" si="11"/>
         <v>183839.2</v>
       </c>
-      <c r="AK60" s="109"/>
-      <c r="AL60" s="107"/>
+      <c r="AK60" s="108"/>
+      <c r="AL60" s="75"/>
       <c r="AM60" s="27">
         <v>48</v>
       </c>
@@ -6176,8 +6145,8 @@
         <f t="shared" si="5"/>
         <v>1320000</v>
       </c>
-      <c r="AE61" s="108"/>
-      <c r="AF61" s="112">
+      <c r="AE61" s="106"/>
+      <c r="AF61" s="77">
         <v>5</v>
       </c>
       <c r="AG61" s="20">
@@ -6194,8 +6163,8 @@
         <f t="shared" si="11"/>
         <v>183757.592</v>
       </c>
-      <c r="AK61" s="109"/>
-      <c r="AL61" s="110">
+      <c r="AK61" s="108"/>
+      <c r="AL61" s="73">
         <v>5</v>
       </c>
       <c r="AM61" s="27">
@@ -6259,8 +6228,8 @@
         <f t="shared" si="5"/>
         <v>1344000</v>
       </c>
-      <c r="AE62" s="108"/>
-      <c r="AF62" s="113"/>
+      <c r="AE62" s="106"/>
+      <c r="AF62" s="78"/>
       <c r="AG62" s="20">
         <v>50</v>
       </c>
@@ -6275,8 +6244,8 @@
         <f t="shared" si="11"/>
         <v>183675.16792000001</v>
       </c>
-      <c r="AK62" s="109"/>
-      <c r="AL62" s="106"/>
+      <c r="AK62" s="108"/>
+      <c r="AL62" s="74"/>
       <c r="AM62" s="27">
         <v>50</v>
       </c>
@@ -6338,8 +6307,8 @@
         <f t="shared" si="5"/>
         <v>1368000</v>
       </c>
-      <c r="AE63" s="108"/>
-      <c r="AF63" s="113"/>
+      <c r="AE63" s="106"/>
+      <c r="AF63" s="78"/>
       <c r="AG63" s="20">
         <v>51</v>
       </c>
@@ -6354,8 +6323,8 @@
         <f t="shared" si="11"/>
         <v>183591.91959919999</v>
       </c>
-      <c r="AK63" s="109"/>
-      <c r="AL63" s="106"/>
+      <c r="AK63" s="108"/>
+      <c r="AL63" s="74"/>
       <c r="AM63" s="27">
         <v>51</v>
       </c>
@@ -6417,8 +6386,8 @@
         <f t="shared" si="5"/>
         <v>1392000</v>
       </c>
-      <c r="AE64" s="108"/>
-      <c r="AF64" s="113"/>
+      <c r="AE64" s="106"/>
+      <c r="AF64" s="78"/>
       <c r="AG64" s="20">
         <v>52</v>
       </c>
@@ -6433,8 +6402,8 @@
         <f t="shared" si="11"/>
         <v>183507.83879519202</v>
       </c>
-      <c r="AK64" s="109"/>
-      <c r="AL64" s="106"/>
+      <c r="AK64" s="108"/>
+      <c r="AL64" s="74"/>
       <c r="AM64" s="27">
         <v>52</v>
       </c>
@@ -6496,8 +6465,8 @@
         <f t="shared" si="5"/>
         <v>1416000</v>
       </c>
-      <c r="AE65" s="108"/>
-      <c r="AF65" s="113"/>
+      <c r="AE65" s="106"/>
+      <c r="AF65" s="78"/>
       <c r="AG65" s="20">
         <v>53</v>
       </c>
@@ -6512,8 +6481,8 @@
         <f t="shared" si="11"/>
         <v>183422.91718314393</v>
       </c>
-      <c r="AK65" s="109"/>
-      <c r="AL65" s="106"/>
+      <c r="AK65" s="108"/>
+      <c r="AL65" s="74"/>
       <c r="AM65" s="27">
         <v>53</v>
       </c>
@@ -6575,8 +6544,8 @@
         <f t="shared" si="5"/>
         <v>1440000</v>
       </c>
-      <c r="AE66" s="108"/>
-      <c r="AF66" s="113"/>
+      <c r="AE66" s="106"/>
+      <c r="AF66" s="78"/>
       <c r="AG66" s="20">
         <v>54</v>
       </c>
@@ -6591,8 +6560,8 @@
         <f t="shared" si="11"/>
         <v>183337.14635497535</v>
       </c>
-      <c r="AK66" s="109"/>
-      <c r="AL66" s="106"/>
+      <c r="AK66" s="108"/>
+      <c r="AL66" s="74"/>
       <c r="AM66" s="27">
         <v>54</v>
       </c>
@@ -6654,8 +6623,8 @@
         <f t="shared" si="5"/>
         <v>1464000</v>
       </c>
-      <c r="AE67" s="108"/>
-      <c r="AF67" s="113"/>
+      <c r="AE67" s="106"/>
+      <c r="AF67" s="78"/>
       <c r="AG67" s="20">
         <v>55</v>
       </c>
@@ -6670,8 +6639,8 @@
         <f t="shared" si="11"/>
         <v>183250.51781852511</v>
       </c>
-      <c r="AK67" s="109"/>
-      <c r="AL67" s="106"/>
+      <c r="AK67" s="108"/>
+      <c r="AL67" s="74"/>
       <c r="AM67" s="27">
         <v>55</v>
       </c>
@@ -6733,8 +6702,8 @@
         <f t="shared" si="5"/>
         <v>1488000</v>
       </c>
-      <c r="AE68" s="108"/>
-      <c r="AF68" s="113"/>
+      <c r="AE68" s="106"/>
+      <c r="AF68" s="78"/>
       <c r="AG68" s="20">
         <v>56</v>
       </c>
@@ -6749,8 +6718,8 @@
         <f t="shared" si="11"/>
         <v>183163.02299671035</v>
       </c>
-      <c r="AK68" s="109"/>
-      <c r="AL68" s="106"/>
+      <c r="AK68" s="108"/>
+      <c r="AL68" s="74"/>
       <c r="AM68" s="27">
         <v>56</v>
       </c>
@@ -6812,8 +6781,8 @@
         <f t="shared" si="5"/>
         <v>1512000</v>
       </c>
-      <c r="AE69" s="108"/>
-      <c r="AF69" s="113"/>
+      <c r="AE69" s="106"/>
+      <c r="AF69" s="78"/>
       <c r="AG69" s="20">
         <v>57</v>
       </c>
@@ -6828,8 +6797,8 @@
         <f t="shared" si="11"/>
         <v>183074.65322667747</v>
       </c>
-      <c r="AK69" s="109"/>
-      <c r="AL69" s="106"/>
+      <c r="AK69" s="108"/>
+      <c r="AL69" s="74"/>
       <c r="AM69" s="27">
         <v>57</v>
       </c>
@@ -6891,8 +6860,8 @@
         <f t="shared" si="5"/>
         <v>1536000</v>
       </c>
-      <c r="AE70" s="108"/>
-      <c r="AF70" s="113"/>
+      <c r="AE70" s="106"/>
+      <c r="AF70" s="78"/>
       <c r="AG70" s="20">
         <v>58</v>
       </c>
@@ -6907,8 +6876,8 @@
         <f t="shared" si="11"/>
         <v>182985.39975894423</v>
       </c>
-      <c r="AK70" s="109"/>
-      <c r="AL70" s="106"/>
+      <c r="AK70" s="108"/>
+      <c r="AL70" s="74"/>
       <c r="AM70" s="27">
         <v>58</v>
       </c>
@@ -6970,8 +6939,8 @@
         <f t="shared" si="5"/>
         <v>1560000</v>
       </c>
-      <c r="AE71" s="108"/>
-      <c r="AF71" s="113"/>
+      <c r="AE71" s="106"/>
+      <c r="AF71" s="78"/>
       <c r="AG71" s="20">
         <v>59</v>
       </c>
@@ -6986,8 +6955,8 @@
         <f t="shared" si="11"/>
         <v>182895.2537565337</v>
       </c>
-      <c r="AK71" s="109"/>
-      <c r="AL71" s="106"/>
+      <c r="AK71" s="108"/>
+      <c r="AL71" s="74"/>
       <c r="AM71" s="27">
         <v>59</v>
       </c>
@@ -7049,8 +7018,8 @@
         <f t="shared" ref="O72:O135" si="25">$W$16*E72</f>
         <v>1584000</v>
       </c>
-      <c r="AE72" s="108"/>
-      <c r="AF72" s="114"/>
+      <c r="AE72" s="106"/>
+      <c r="AF72" s="79"/>
       <c r="AG72" s="20">
         <v>60</v>
       </c>
@@ -7065,8 +7034,8 @@
         <f t="shared" si="11"/>
         <v>182804.20629409901</v>
       </c>
-      <c r="AK72" s="109"/>
-      <c r="AL72" s="111"/>
+      <c r="AK72" s="108"/>
+      <c r="AL72" s="76"/>
       <c r="AM72" s="28">
         <v>60</v>
       </c>
@@ -7128,12 +7097,12 @@
         <f t="shared" si="25"/>
         <v>1608000</v>
       </c>
-      <c r="AM73" s="79" t="s">
+      <c r="AM73" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="AN73" s="79"/>
-      <c r="AO73" s="79"/>
-      <c r="AP73" s="79"/>
+      <c r="AN73" s="111"/>
+      <c r="AO73" s="111"/>
+      <c r="AP73" s="111"/>
     </row>
     <row r="74" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C74" s="46">
@@ -7181,10 +7150,10 @@
         <f t="shared" si="25"/>
         <v>1632000</v>
       </c>
-      <c r="AM74" s="73"/>
-      <c r="AN74" s="73"/>
-      <c r="AO74" s="73"/>
-      <c r="AP74" s="73"/>
+      <c r="AM74" s="112"/>
+      <c r="AN74" s="112"/>
+      <c r="AO74" s="112"/>
+      <c r="AP74" s="112"/>
     </row>
     <row r="75" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="46">
@@ -7232,10 +7201,10 @@
         <f t="shared" si="25"/>
         <v>1656000</v>
       </c>
-      <c r="AM75" s="73"/>
-      <c r="AN75" s="73"/>
-      <c r="AO75" s="73"/>
-      <c r="AP75" s="73"/>
+      <c r="AM75" s="112"/>
+      <c r="AN75" s="112"/>
+      <c r="AO75" s="112"/>
+      <c r="AP75" s="112"/>
     </row>
     <row r="76" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="46">
@@ -7283,10 +7252,10 @@
         <f t="shared" si="25"/>
         <v>1680000</v>
       </c>
-      <c r="AM76" s="73"/>
-      <c r="AN76" s="73"/>
-      <c r="AO76" s="73"/>
-      <c r="AP76" s="73"/>
+      <c r="AM76" s="112"/>
+      <c r="AN76" s="112"/>
+      <c r="AO76" s="112"/>
+      <c r="AP76" s="112"/>
     </row>
     <row r="77" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="46">
@@ -7334,10 +7303,10 @@
         <f t="shared" si="25"/>
         <v>1704000</v>
       </c>
-      <c r="AM77" s="73"/>
-      <c r="AN77" s="73"/>
-      <c r="AO77" s="73"/>
-      <c r="AP77" s="73"/>
+      <c r="AM77" s="112"/>
+      <c r="AN77" s="112"/>
+      <c r="AO77" s="112"/>
+      <c r="AP77" s="112"/>
     </row>
     <row r="78" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C78" s="46">
@@ -7385,15 +7354,15 @@
         <f t="shared" si="25"/>
         <v>1728000</v>
       </c>
-      <c r="AM78" s="73" t="s">
+      <c r="AM78" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="AN78" s="73"/>
-      <c r="AO78" s="77">
+      <c r="AN78" s="112"/>
+      <c r="AO78" s="113">
         <f>SUM(AP13:AP72)</f>
         <v>8880109.1319320202</v>
       </c>
-      <c r="AP78" s="77"/>
+      <c r="AP78" s="113"/>
     </row>
     <row r="79" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="46">
@@ -7441,10 +7410,10 @@
         <f t="shared" si="25"/>
         <v>1752000</v>
       </c>
-      <c r="AM79" s="73"/>
-      <c r="AN79" s="73"/>
-      <c r="AO79" s="77"/>
-      <c r="AP79" s="77"/>
+      <c r="AM79" s="112"/>
+      <c r="AN79" s="112"/>
+      <c r="AO79" s="113"/>
+      <c r="AP79" s="113"/>
     </row>
     <row r="80" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="46">
@@ -7492,10 +7461,10 @@
         <f t="shared" si="25"/>
         <v>1776000</v>
       </c>
-      <c r="AM80" s="73"/>
-      <c r="AN80" s="73"/>
-      <c r="AO80" s="77"/>
-      <c r="AP80" s="77"/>
+      <c r="AM80" s="112"/>
+      <c r="AN80" s="112"/>
+      <c r="AO80" s="113"/>
+      <c r="AP80" s="113"/>
     </row>
     <row r="81" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="46">
@@ -7543,10 +7512,10 @@
         <f t="shared" si="25"/>
         <v>1800000</v>
       </c>
-      <c r="AM81" s="73"/>
-      <c r="AN81" s="73"/>
-      <c r="AO81" s="77"/>
-      <c r="AP81" s="77"/>
+      <c r="AM81" s="112"/>
+      <c r="AN81" s="112"/>
+      <c r="AO81" s="113"/>
+      <c r="AP81" s="113"/>
     </row>
     <row r="82" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C82" s="46">
@@ -7594,15 +7563,15 @@
         <f t="shared" si="25"/>
         <v>1824000</v>
       </c>
-      <c r="AM82" s="75" t="s">
+      <c r="AM82" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="AN82" s="75"/>
-      <c r="AO82" s="76">
+      <c r="AN82" s="109"/>
+      <c r="AO82" s="110">
         <f>-(SUM('[1]gestion emprunt'!J9:J10))</f>
         <v>-170000</v>
       </c>
-      <c r="AP82" s="76"/>
+      <c r="AP82" s="110"/>
     </row>
     <row r="83" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C83" s="46">
@@ -7650,10 +7619,10 @@
         <f t="shared" si="25"/>
         <v>1848000</v>
       </c>
-      <c r="AM83" s="75"/>
-      <c r="AN83" s="75"/>
-      <c r="AO83" s="76"/>
-      <c r="AP83" s="76"/>
+      <c r="AM83" s="109"/>
+      <c r="AN83" s="109"/>
+      <c r="AO83" s="110"/>
+      <c r="AP83" s="110"/>
     </row>
     <row r="84" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C84" s="46">
@@ -7701,10 +7670,10 @@
         <f t="shared" si="25"/>
         <v>1872000</v>
       </c>
-      <c r="AM84" s="75"/>
-      <c r="AN84" s="75"/>
-      <c r="AO84" s="76"/>
-      <c r="AP84" s="76"/>
+      <c r="AM84" s="109"/>
+      <c r="AN84" s="109"/>
+      <c r="AO84" s="110"/>
+      <c r="AP84" s="110"/>
     </row>
     <row r="85" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C85" s="46">
@@ -7752,15 +7721,15 @@
         <f t="shared" si="25"/>
         <v>1896000</v>
       </c>
-      <c r="AM85" s="73" t="s">
+      <c r="AM85" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="AN85" s="73"/>
-      <c r="AO85" s="77">
+      <c r="AN85" s="112"/>
+      <c r="AO85" s="113">
         <f>AO78-ABS(AO82)</f>
         <v>8710109.1319320202</v>
       </c>
-      <c r="AP85" s="77"/>
+      <c r="AP85" s="113"/>
     </row>
     <row r="86" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C86" s="46">
@@ -7808,10 +7777,10 @@
         <f t="shared" si="25"/>
         <v>1920000</v>
       </c>
-      <c r="AM86" s="73"/>
-      <c r="AN86" s="73"/>
-      <c r="AO86" s="77"/>
-      <c r="AP86" s="77"/>
+      <c r="AM86" s="112"/>
+      <c r="AN86" s="112"/>
+      <c r="AO86" s="113"/>
+      <c r="AP86" s="113"/>
     </row>
     <row r="87" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="46">
@@ -7859,10 +7828,10 @@
         <f t="shared" si="25"/>
         <v>1944000</v>
       </c>
-      <c r="AM87" s="73"/>
-      <c r="AN87" s="73"/>
-      <c r="AO87" s="77"/>
-      <c r="AP87" s="77"/>
+      <c r="AM87" s="112"/>
+      <c r="AN87" s="112"/>
+      <c r="AO87" s="113"/>
+      <c r="AP87" s="113"/>
     </row>
     <row r="88" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="46">
@@ -7910,10 +7879,10 @@
         <f t="shared" si="25"/>
         <v>1968000</v>
       </c>
-      <c r="AM88" s="73"/>
-      <c r="AN88" s="73"/>
-      <c r="AO88" s="77"/>
-      <c r="AP88" s="77"/>
+      <c r="AM88" s="112"/>
+      <c r="AN88" s="112"/>
+      <c r="AO88" s="113"/>
+      <c r="AP88" s="113"/>
     </row>
     <row r="89" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="46">
@@ -7961,15 +7930,15 @@
         <f t="shared" si="25"/>
         <v>1992000</v>
       </c>
-      <c r="AM89" s="75" t="s">
+      <c r="AM89" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="AN89" s="75"/>
-      <c r="AO89" s="76">
+      <c r="AN89" s="109"/>
+      <c r="AO89" s="110">
         <f>-77000</f>
         <v>-77000</v>
       </c>
-      <c r="AP89" s="76"/>
+      <c r="AP89" s="110"/>
     </row>
     <row r="90" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="46">
@@ -8017,10 +7986,10 @@
         <f t="shared" si="25"/>
         <v>2016000</v>
       </c>
-      <c r="AM90" s="75"/>
-      <c r="AN90" s="75"/>
-      <c r="AO90" s="76"/>
-      <c r="AP90" s="76"/>
+      <c r="AM90" s="109"/>
+      <c r="AN90" s="109"/>
+      <c r="AO90" s="110"/>
+      <c r="AP90" s="110"/>
     </row>
     <row r="91" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="46">
@@ -8068,10 +8037,10 @@
         <f t="shared" si="25"/>
         <v>2040000</v>
       </c>
-      <c r="AM91" s="75"/>
-      <c r="AN91" s="75"/>
-      <c r="AO91" s="76"/>
-      <c r="AP91" s="76"/>
+      <c r="AM91" s="109"/>
+      <c r="AN91" s="109"/>
+      <c r="AO91" s="110"/>
+      <c r="AP91" s="110"/>
     </row>
     <row r="92" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="46">
@@ -8119,10 +8088,10 @@
         <f t="shared" si="25"/>
         <v>2064000</v>
       </c>
-      <c r="AO92" s="73" t="s">
+      <c r="AO92" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="AP92" s="74">
+      <c r="AP92" s="114">
         <f>AO85-ABS(AO89)</f>
         <v>8633109.1319320202</v>
       </c>
@@ -8173,8 +8142,8 @@
         <f t="shared" si="25"/>
         <v>2088000</v>
       </c>
-      <c r="AO93" s="73"/>
-      <c r="AP93" s="74"/>
+      <c r="AO93" s="112"/>
+      <c r="AP93" s="114"/>
     </row>
     <row r="94" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C94" s="46">
@@ -8222,8 +8191,8 @@
         <f t="shared" si="25"/>
         <v>2112000</v>
       </c>
-      <c r="AO94" s="73"/>
-      <c r="AP94" s="74"/>
+      <c r="AO94" s="112"/>
+      <c r="AP94" s="114"/>
     </row>
     <row r="95" spans="3:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C95" s="46">
@@ -8271,8 +8240,8 @@
         <f t="shared" si="25"/>
         <v>2136000</v>
       </c>
-      <c r="AO95" s="73"/>
-      <c r="AP95" s="74"/>
+      <c r="AO95" s="112"/>
+      <c r="AP95" s="114"/>
     </row>
     <row r="96" spans="3:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C96" s="46">
@@ -12056,11 +12025,18 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AL25:AL36"/>
-    <mergeCell ref="AL37:AL48"/>
-    <mergeCell ref="AL49:AL60"/>
-    <mergeCell ref="AL61:AL72"/>
-    <mergeCell ref="AF61:AF72"/>
+    <mergeCell ref="AO92:AO95"/>
+    <mergeCell ref="AP92:AP95"/>
+    <mergeCell ref="AM89:AN91"/>
+    <mergeCell ref="AO89:AP91"/>
+    <mergeCell ref="AM85:AN88"/>
+    <mergeCell ref="AO85:AP88"/>
+    <mergeCell ref="AM82:AN84"/>
+    <mergeCell ref="AO82:AP84"/>
+    <mergeCell ref="AF49:AF60"/>
+    <mergeCell ref="AM73:AP77"/>
+    <mergeCell ref="AM78:AN81"/>
+    <mergeCell ref="AO78:AP81"/>
     <mergeCell ref="U12:U16"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="U3:W3"/>
@@ -12077,18 +12053,11 @@
     <mergeCell ref="AK13:AK72"/>
     <mergeCell ref="AF25:AF36"/>
     <mergeCell ref="AF37:AF48"/>
-    <mergeCell ref="AM82:AN84"/>
-    <mergeCell ref="AO82:AP84"/>
-    <mergeCell ref="AF49:AF60"/>
-    <mergeCell ref="AM73:AP77"/>
-    <mergeCell ref="AM78:AN81"/>
-    <mergeCell ref="AO78:AP81"/>
-    <mergeCell ref="AO92:AO95"/>
-    <mergeCell ref="AP92:AP95"/>
-    <mergeCell ref="AM89:AN91"/>
-    <mergeCell ref="AO89:AP91"/>
-    <mergeCell ref="AM85:AN88"/>
-    <mergeCell ref="AO85:AP88"/>
+    <mergeCell ref="AL25:AL36"/>
+    <mergeCell ref="AL37:AL48"/>
+    <mergeCell ref="AL49:AL60"/>
+    <mergeCell ref="AL61:AL72"/>
+    <mergeCell ref="AF61:AF72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>